<commit_message>
allow unused cameras to pass through
</commit_message>
<xml_diff>
--- a/in/apr14T085430.xlsx
+++ b/in/apr14T085430.xlsx
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="101">
   <si>
     <t xml:space="preserve">Sim</t>
   </si>
@@ -365,6 +365,9 @@
   </si>
   <si>
     <t xml:space="preserve">2013-04-14T8-54_hst1.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~/Dropbox/aurora_data/StudyEvents/2013-04-14/DASC/raw</t>
   </si>
   <si>
     <t xml:space="preserve">plotMinVal</t>
@@ -691,7 +694,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="53">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -896,14 +899,6 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1000,13 +995,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.030612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.6122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.93367346938776"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.26530612244898"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.15816326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.484693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.8112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1607,15 +1602,16 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="41" width="18.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="41" width="26.3520408163265"/>
-    <col collapsed="false" hidden="false" max="251" min="4" style="41" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="252" style="0" width="8.53061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="41" width="18.6836734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="41" width="23.280612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="41" width="18.25"/>
+    <col collapsed="false" hidden="false" max="251" min="5" style="41" width="8.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="252" style="0" width="8.63775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1626,7 +1622,9 @@
       <c r="C1" s="42" t="n">
         <v>1</v>
       </c>
-      <c r="D1" s="0"/>
+      <c r="D1" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="E1" s="0"/>
       <c r="F1" s="0"/>
       <c r="G1" s="0"/>
@@ -1885,7 +1883,9 @@
       <c r="C2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="0"/>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="E2" s="0"/>
       <c r="F2" s="0"/>
       <c r="G2" s="0"/>
@@ -3439,7 +3439,9 @@
       <c r="C8" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="0"/>
+      <c r="D8" s="0" t="s">
+        <v>83</v>
+      </c>
       <c r="E8" s="0"/>
       <c r="F8" s="0"/>
       <c r="G8" s="0"/>
@@ -3943,7 +3945,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B10" s="49" t="n">
         <v>10</v>
@@ -4202,7 +4204,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B11" s="49" t="n">
         <v>35000</v>
@@ -4461,13 +4463,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B12" s="51" t="n">
+        <v>86</v>
+      </c>
+      <c r="B12" s="4" t="n">
         <f aca="false">1/12</f>
         <v>0.0833333333333333</v>
       </c>
-      <c r="C12" s="52" t="n">
+      <c r="C12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D12" s="0"/>
@@ -4721,7 +4723,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B13" s="0"/>
       <c r="C13" s="0"/>
@@ -4976,7 +4978,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1750</v>
@@ -5488,7 +5490,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B16" s="5" t="n">
         <v>15</v>
@@ -5747,7 +5749,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B17" s="5" t="n">
         <v>2</v>
@@ -6011,7 +6013,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B19" s="4" t="n">
         <v>77.51</v>
@@ -6022,7 +6024,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B20" s="4" t="n">
         <v>19.92</v>
@@ -6033,24 +6035,24 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6059,21 +6061,21 @@
       <c r="C23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="53" t="s">
-        <v>97</v>
-      </c>
-      <c r="B24" s="54" t="n">
+      <c r="A24" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="52" t="n">
         <f aca="false">(0.0016)^2</f>
         <v>2.56E-006</v>
       </c>
-      <c r="C24" s="54" t="n">
+      <c r="C24" s="52" t="n">
         <f aca="false">(0.0016)^2</f>
         <v>2.56E-006</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="53" t="s">
-        <v>98</v>
+      <c r="A25" s="51" t="s">
+        <v>99</v>
       </c>
       <c r="B25" s="41" t="n">
         <v>1</v>
@@ -6083,8 +6085,8 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="53" t="s">
-        <v>99</v>
+      <c r="A26" s="51" t="s">
+        <v>100</v>
       </c>
       <c r="B26" s="41" t="n">
         <v>200</v>

</xml_diff>

<commit_message>
only load eigenprofile if doing inversion
</commit_message>
<xml_diff>
--- a/in/apr14T085430.xlsx
+++ b/in/apr14T085430.xlsx
@@ -268,13 +268,13 @@
     <t xml:space="preserve">reqStartUT</t>
   </si>
   <si>
-    <t xml:space="preserve">2013-04-14T08:54:30.500Z</t>
+    <t xml:space="preserve">2013-04-14T08:54:28Z</t>
   </si>
   <si>
     <t xml:space="preserve">reqStopUT</t>
   </si>
   <si>
-    <t xml:space="preserve">2013-04-14T08:54:30.800Z</t>
+    <t xml:space="preserve">2013-04-14T08:54:35Z</t>
   </si>
   <si>
     <t xml:space="preserve">UseTCz</t>
@@ -697,7 +697,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -902,6 +902,10 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -991,20 +995,20 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
+      <selection pane="bottomLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.6122448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.93367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.26530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.15816326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.8112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1605,16 +1609,16 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="41" width="18.6836734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="41" width="23.280612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="41" width="18.25"/>
-    <col collapsed="false" hidden="false" max="251" min="5" style="41" width="8.75"/>
-    <col collapsed="false" hidden="false" max="1025" min="252" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="41" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="41" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="41" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="251" min="5" style="41" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="252" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3956,7 +3960,9 @@
       <c r="C10" s="50" t="n">
         <v>1000</v>
       </c>
-      <c r="D10" s="0"/>
+      <c r="D10" s="0" t="n">
+        <v>300</v>
+      </c>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
@@ -4210,12 +4216,15 @@
         <v>86</v>
       </c>
       <c r="B11" s="49" t="n">
-        <v>35000</v>
-      </c>
-      <c r="C11" s="50" t="n">
-        <v>2500</v>
-      </c>
-      <c r="D11" s="0"/>
+        <v>50000</v>
+      </c>
+      <c r="C11" s="51" t="n">
+        <f aca="false">B11*B12</f>
+        <v>4166.66666666667</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>1000</v>
+      </c>
       <c r="E11" s="0"/>
       <c r="F11" s="0"/>
       <c r="G11" s="0"/>
@@ -6064,20 +6073,20 @@
       <c r="C23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="51" t="s">
+      <c r="A24" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="B24" s="52" t="n">
+      <c r="B24" s="53" t="n">
         <f aca="false">(0.0016)^2</f>
         <v>2.56E-006</v>
       </c>
-      <c r="C24" s="52" t="n">
+      <c r="C24" s="53" t="n">
         <f aca="false">(0.0016)^2</f>
         <v>2.56E-006</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="51" t="s">
+      <c r="A25" s="52" t="s">
         <v>100</v>
       </c>
       <c r="B25" s="41" t="n">
@@ -6088,7 +6097,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="51" t="s">
+      <c r="A26" s="52" t="s">
         <v>101</v>
       </c>
       <c r="B26" s="41" t="n">

</xml_diff>

<commit_message>
prepare to make common fov overlay
</commit_message>
<xml_diff>
--- a/in/apr14T085430.xlsx
+++ b/in/apr14T085430.xlsx
@@ -98,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A25" authorId="0">
+    <comment ref="A27" authorId="0">
       <text>
         <r>
           <rPr>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="106">
   <si>
     <t xml:space="preserve">Sim</t>
   </si>
@@ -268,13 +268,13 @@
     <t xml:space="preserve">reqStartUT</t>
   </si>
   <si>
-    <t xml:space="preserve">2013-04-14T08:54:28Z</t>
+    <t xml:space="preserve">2013-04-14T08:54:30.500Z</t>
   </si>
   <si>
     <t xml:space="preserve">reqStopUT</t>
   </si>
   <si>
-    <t xml:space="preserve">2013-04-14T08:54:35Z</t>
+    <t xml:space="preserve">2013-04-14T08:54:30.800Z</t>
   </si>
   <si>
     <t xml:space="preserve">UseTCz</t>
@@ -413,6 +413,18 @@
   </si>
   <si>
     <t xml:space="preserve">hst1cal.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">azcalfn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../dascutils/cal/PKR_DASC_20110112_AZ_10deg.fits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elcalfn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../dascutils/cal/PKR_DASC_20110112_EL_10deg.fits</t>
   </si>
   <si>
     <t xml:space="preserve">pixarea_sqcm</t>
@@ -995,20 +1007,20 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
+      <selection pane="bottomLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.6122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.93367346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.26530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.15816326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.8112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1604,21 +1616,21 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IQ26"/>
+  <dimension ref="A1:IQ28"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="41" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="41" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="41" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="251" min="5" style="41" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="252" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="41" width="18.6836734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="41" width="23.280612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="41" width="18.25"/>
+    <col collapsed="false" hidden="false" max="251" min="5" style="41" width="8.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="252" style="0" width="8.63775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3961,7 +3973,7 @@
         <v>1000</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
@@ -4219,11 +4231,11 @@
         <v>50000</v>
       </c>
       <c r="C11" s="51" t="n">
-        <f aca="false">B11*B12</f>
+        <f aca="false">B12*B11</f>
         <v>4166.66666666667</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="E11" s="0"/>
       <c r="F11" s="0"/>
@@ -6068,42 +6080,62 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0"/>
-      <c r="B23" s="0"/>
-      <c r="C23" s="0"/>
+      <c r="A23" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="41" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="52" t="s">
-        <v>99</v>
-      </c>
-      <c r="B24" s="53" t="n">
+      <c r="A24" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0"/>
+      <c r="B25" s="0"/>
+      <c r="C25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="52" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="53" t="n">
         <f aca="false">(0.0016)^2</f>
         <v>2.56E-006</v>
       </c>
-      <c r="C24" s="53" t="n">
+      <c r="C26" s="53" t="n">
         <f aca="false">(0.0016)^2</f>
         <v>2.56E-006</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="52" t="s">
-        <v>100</v>
-      </c>
-      <c r="B25" s="41" t="n">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="52" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" s="41" t="n">
         <v>1</v>
       </c>
-      <c r="C25" s="41" t="n">
+      <c r="C27" s="41" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="52" t="s">
-        <v>101</v>
-      </c>
-      <c r="B26" s="41" t="n">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="52" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="41" t="n">
         <v>200</v>
       </c>
-      <c r="C26" s="41" t="n">
+      <c r="C28" s="41" t="n">
         <v>200</v>
       </c>
     </row>

</xml_diff>

<commit_message>
in progress ini instead of xls
</commit_message>
<xml_diff>
--- a/in/apr14T085430.xlsx
+++ b/in/apr14T085430.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sim" sheetId="1" state="visible" r:id="rId2"/>
@@ -274,13 +274,13 @@
     <t xml:space="preserve">reqStartUT</t>
   </si>
   <si>
-    <t xml:space="preserve">2013-04-14T08:54:20Z</t>
+    <t xml:space="preserve">2013-04-14T08:54:27.95Z</t>
   </si>
   <si>
     <t xml:space="preserve">reqStopUT</t>
   </si>
   <si>
-    <t xml:space="preserve">2013-04-14T08:54:40Z</t>
+    <t xml:space="preserve">2013-04-14T08:54:27.97Z</t>
   </si>
   <si>
     <t xml:space="preserve">UseTCz</t>
@@ -1009,19 +1009,19 @@
   <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.44897959183673"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1637,11 +1637,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="41" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="41" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="41" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="251" min="5" style="41" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="252" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="41" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="41" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="41" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="251" min="5" style="41" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="252" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>